<commit_message>
reorganized to have separate functions for SequenceMatcher and NLP. The program runs through SequenceMatcher first and then run through NLP for rows that are less than 1. The program also splits the table into separate tables to run through the whole table concurrently, then combines it back together. It then outputs the full dataset with standardized job titles and job descriptions. Need to look into what score tolerance to allow when clustering and analyzing. Also need to look into the job description data to see how accurate they are.
</commit_message>
<xml_diff>
--- a/output/Standardized Job Titles and SOC Codes_6.xlsx
+++ b/output/Standardized Job Titles and SOC Codes_6.xlsx
@@ -476,12 +476,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Score</t>
+          <t>SOC Code</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>SOC Code</t>
+          <t>Match Score</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -523,13 +523,13 @@
           <t>Digital Court Reporter</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>27-3092.00</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
         <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>27-3092.00</t>
-        </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -570,13 +570,13 @@
           <t>Legal Administrator</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>23-2099.00</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
         <v>1</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>23-2099.00</t>
-        </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -617,13 +617,13 @@
           <t>Legal Clerk</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>23-1012.00</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
         <v>1</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>23-1012.00</t>
-        </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>

</xml_diff>